<commit_message>
Feat 59: Include address scrapping
</commit_message>
<xml_diff>
--- a/59.themeparks/extracted_data/59.Data.xlsx
+++ b/59.themeparks/extracted_data/59.Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="201">
   <si>
     <t>title</t>
   </si>
@@ -29,6 +29,9 @@
     <t>mapLink</t>
   </si>
   <si>
+    <t>Address</t>
+  </si>
+  <si>
     <t>Adventure Island</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
     <t>https://maps.google.co.uk/maps?q=adventure+island&amp;oe=utf-8&amp;client=firefox-a&amp;channel=sb&amp;ie=UTF8&amp;hq=&amp;hnear=&amp;ll=51.532394,0.716916&amp;spn=0.006295,0.006295&amp;t=h&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>Adventure Island, Western Esplanade, Southend-on-Sea SS1 1EE, United Kingdom</t>
+  </si>
+  <si>
     <t>Adventure Wonderland</t>
   </si>
   <si>
@@ -53,6 +59,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d1623.3048089362055!2d-1.8452566424510355!3d50.775162471816984!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x487398e13af9a715%3A0x15f1acb138e4c5a8!2sAdventure+Wonderland!5e1!3m2!1sen!2suk!4v1494175585303</t>
   </si>
   <si>
+    <t>Adventure Wonderland, Merritown Ln, Hurn, Christchurch BH23 6BA</t>
+  </si>
+  <si>
     <t>Barry Island Pleasure Park</t>
   </si>
   <si>
@@ -65,6 +74,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d1913.486885623704!2d-3.2750949154006492!3d51.39158536926824!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x486e05fb74864843%3A0x5cda027fb5f8598a!2sBarry%20Island%20Pleasure%20Park!5e1!3m2!1sen!2suk!4v1654774933306!5m2!1sen!2suk</t>
   </si>
   <si>
+    <t>Barry Island Pleasure Park, Friars Rd, Barry CF62 5TR</t>
+  </si>
+  <si>
     <t>Blackgang Chine</t>
   </si>
   <si>
@@ -77,6 +89,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d12124.819664919756!2d-1.3241666224068014!3d50.587154619504126!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x4874867566985967%3A0xed49f3c58b269383!2sBlackgang%20Chine!5e1!3m2!1sen!2suk!4v1708604726771!5m2!1sen!2suk</t>
   </si>
   <si>
+    <t>Blackgang Chine, Ventnor PO38 2HN</t>
+  </si>
+  <si>
     <t>Brean Theme Park</t>
   </si>
   <si>
@@ -89,6 +104,9 @@
     <t>https://maps.google.co.uk/maps?q=brean+leisure+park&amp;oe=utf-8&amp;client=firefox-a&amp;channel=sb&amp;ie=UTF8&amp;hq=&amp;hnear=&amp;ll=51.285462,-3.010563&amp;spn=0.006295,0.006295&amp;t=h&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>Brean Leisure Park, Richard's Wy, Brean, Burnham-on-Sea TA8 2RA, United Kingdom</t>
+  </si>
+  <si>
     <t>Camel Creek Family Adventure Park</t>
   </si>
   <si>
@@ -101,6 +119,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d2261.8168400715936!2d-4.931790660061178!3d50.48877954234847!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x486b749f6e9a74d1%3A0xaadb28c7bc9cf6c1!2sCamel+Creek+Adventure+Park!5e1!3m2!1sen!2suk!4v1476895237819</t>
   </si>
   <si>
+    <t>Camel Creek Family Adventure Park, Tredinnick, Wadebridge PL27 7RA</t>
+  </si>
+  <si>
     <t>Codonas</t>
   </si>
   <si>
@@ -110,6 +131,9 @@
     <t>Codonas in Aberdeen offers a wide range of fun with all its rides and attractions including – two roller coasters - The Looping Star and The Apple Family Coaster, and the Disco Waltzers, Super Dodgems, White Water Log Flume, Vertigo Aerial Assault Course, Animal Barn Pet Centre, Super Trucks and Smugglers Cove.</t>
   </si>
   <si>
+    <t>Address not found</t>
+  </si>
+  <si>
     <t>Crealy Theme Park &amp; Resort</t>
   </si>
   <si>
@@ -143,6 +167,9 @@
     <t>https://googleads.g.doubleclick.net/pagead/ads?gdpr=0&amp;client=ca-pub-1049321617959519&amp;output=html&amp;h=250&amp;adk=2338749149&amp;adf=4280107306&amp;pi=t.aa~a.3566183849~rp.4&amp;w=690&amp;abgtt=6&amp;fwrn=4&amp;fwrnh=100&amp;lmt=1715814080&amp;rafmt=1&amp;to=qs&amp;pwprc=6765933657&amp;format=690x250&amp;url=https%3A%2F%2Fwww.themeparks-uk.com%2Fuk-theme-parks%2Fengland%2Fdreamland-margate&amp;fwr=0&amp;pra=3&amp;rpe=1&amp;resp_fmts=3&amp;wgl=1&amp;fa=40&amp;uach=WyJXaW5kb3dzIiwiMTUuMC4wIiwieDg2IiwiIiwiMTI0LjAuNjM2Ny45MSIsbnVsbCwwLG51bGwsIjY0IixbWyJOb3QtQS5CcmFuZCIsIjk5LjAuMC4wIl0sWyJDaHJvbWl1bSIsIjEyNC4wLjYzNjcuOTEiXV0sMF0.&amp;dt=1715814079603&amp;bpp=1&amp;bdt=8844&amp;idt=-M&amp;shv=r20240513&amp;mjsv=m202405080101&amp;ptt=9&amp;saldr=aa&amp;abxe=1&amp;cookie_enabled=1&amp;eo_id_str=ID%3D9e805196f7a79a49%3AT%3D1715810615%3ART%3D1715810615%3AS%3DAA-AfjYmPms0afe3olUzdZ03Ci7N&amp;prev_fmts=0x0%2C345x280%2C720x280&amp;nras=3&amp;correlator=2761162966898&amp;frm=20&amp;pv=1&amp;ga_vid=592203439.1715814077&amp;ga_sid=1715814079&amp;ga_hid=1742559550&amp;ga_fc=1&amp;u_tz=120&amp;u_his=2&amp;u_h=864&amp;u_w=1536&amp;u_ah=864&amp;u_aw=1536&amp;u_cd=24&amp;u_sd=1&amp;dmc=8&amp;adx=55&amp;ady=1462&amp;biw=800&amp;bih=600&amp;scr_x=0&amp;scr_y=0&amp;eid=44759875%2C44759926%2C44759837%2C31083588%2C95331982%2C31083538%2C95331711%2C95332416%2C31078663%2C31078665%2C31078668%2C31078670&amp;oid=2&amp;psts=AOrYGsnJPCX3y32gyCvH6fUS1UIgbaHZaaRYQPIuRU0j_awRnroUryalFL8q7WjsGZMkpexhvCyEL2fwb8raRR3hkgk&amp;pvsid=1475331653617804&amp;tmod=389228844&amp;uas=0&amp;nvt=1&amp;fc=1920&amp;brdim=12%2C12%2C12%2C12%2C1536%2C0%2C1313%2C996%2C800%2C600&amp;vis=1&amp;rsz=%7C%7Cs%7C&amp;abl=NS&amp;fu=128&amp;bc=31&amp;bz=1.64&amp;td=1&amp;psd=W251bGwsbnVsbCxudWxsLDFd&amp;nt=1&amp;ifi=4&amp;uci=a!4&amp;btvi=2&amp;fsb=1&amp;dtd=1205</t>
   </si>
   <si>
+    <t>Dreamland Margate, 49-51, Marine Terrace, Margate CT9 1XJ</t>
+  </si>
+  <si>
     <t>Drusillas Park</t>
   </si>
   <si>
@@ -164,6 +191,9 @@
     <t>https://maps.google.co.uk/maps?q=fantasy+island&amp;oe=utf-8&amp;client=firefox-a&amp;channel=sb&amp;ie=UTF8&amp;hq=fantasy+island&amp;ll=53.1925,0.349834&amp;spn=0.007752,0.021136&amp;t=h&amp;z=14&amp;iwloc=A&amp;cid=9664714470081121772&amp;output=embed</t>
   </si>
   <si>
+    <t>Fantasy Island, Sea Ln, Ingoldmells, Skegness PE25 1RH, United Kingdom</t>
+  </si>
+  <si>
     <t>Flambards</t>
   </si>
   <si>
@@ -176,6 +206,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d2366.3731379260084!2d-5.260766684430941!3d50.09222977942753!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x486b278e29e0d79b%3A0xabc5ab6710579c07!2sFlambards!5e1!3m2!1sen!2suk!4v1494176817238</t>
   </si>
   <si>
+    <t>Flambards Theme Park, Clodgey Ln, Helston TR13 0QA</t>
+  </si>
+  <si>
     <t>Flamingo Land</t>
   </si>
   <si>
@@ -188,6 +221,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d8008.321275583981!2d-0.8080010769104273!3d54.21155201430274!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x487f29c9df693dd5%3A0xcdd704370d7e0895!2sFlamingo+Land!5e1!3m2!1sen!2suk!4v1427050973677</t>
   </si>
   <si>
+    <t>Flamingo Land Resort, Kirby Misperton, Malton</t>
+  </si>
+  <si>
     <t>Funland Hayling Island</t>
   </si>
   <si>
@@ -209,6 +245,9 @@
     <t>https://maps.google.co.uk/maps?q=great+yarmouth+pleasure+beach&amp;oe=utf-8&amp;client=firefox-a&amp;channel=sb&amp;ie=UTF8&amp;hq=&amp;hnear=&amp;ll=52.592854,1.735954&amp;spn=0.006295,0.006295&amp;t=h&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>Great Yarmouth Pleasure Beach, The Pleasure Beach, S Beach Parade, Great Yarmouth NR30 3EH, United Kingdom</t>
+  </si>
+  <si>
     <t>GreenWood</t>
   </si>
   <si>
@@ -221,6 +260,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d114776.0727158108!2d-4.262250796405382!3d53.19167951630547!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x4865a8fded64d0d7%3A0x58b22bdb55761cee!2sGreenWood%20Family%20Park!5e1!3m2!1sen!2suk!4v1618493211378!5m2!1sen!2suk</t>
   </si>
   <si>
+    <t>GreenWood Family Park, Bush Rd, Y Felinheli LL56 4QN</t>
+  </si>
+  <si>
     <t>Gulliver's Kingdom</t>
   </si>
   <si>
@@ -233,6 +275,9 @@
     <t>https://maps.google.co.uk/maps?oe=utf-8&amp;client=firefox-a&amp;channel=sb&amp;q=Gulliver%27s+Kingdom&amp;ie=UTF8&amp;hq=&amp;hnear=&amp;ll=53.11906,-1.564061&amp;spn=0.006295,0.006295&amp;t=h&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>Gulliver's Kingdom, Temple Walk, Matlock Bath DE4 3PG, United Kingdom</t>
+  </si>
+  <si>
     <t>Gulliver's Land</t>
   </si>
   <si>
@@ -257,6 +302,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d5054.003346502091!2d-1.3099907948077798!3d53.34730939645956!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x48799f959d257d91%3A0xbad476a74ebdd8fd!2sGulliver%27s%20Valley!5e1!3m2!1sen!2suk!4v1593447457282!5m2!1sen!2suk</t>
   </si>
   <si>
+    <t>Gulliver's Valley Theme Park, Mansfield Rd, Sheffield S26 5QW</t>
+  </si>
+  <si>
     <t>Gulliver's World</t>
   </si>
   <si>
@@ -269,6 +317,9 @@
     <t>https://maps.google.co.uk/maps?q=Gulliver%27s+World&amp;oe=utf-8&amp;client=firefox-a&amp;channel=sb&amp;ie=UTF8&amp;hq=&amp;hnear=&amp;ll=53.405656,-2.617654&amp;spn=0.006295,0.006295&amp;t=h&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>Gulliver's World Theme Park, Shackleton Cl, Old Hall, Warrington WA5 9YZ, United Kingdom</t>
+  </si>
+  <si>
     <t>Harbour Park</t>
   </si>
   <si>
@@ -281,6 +332,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d4906.381293957234!2d-0.5441835398324611!3d50.80380252741568!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x4875a5781b4dd45b%3A0x2a994b3dad5cf631!2sHarbour%20Park%20Amusements!5e1!3m2!1sen!2suk!4v1601922933120!5m2!1sen!2suk</t>
   </si>
   <si>
+    <t>Harbour Park Amusements, Windmill Rd, Littlehampton BN17 5LH</t>
+  </si>
+  <si>
     <t>Hyde Park Winter Wonderland</t>
   </si>
   <si>
@@ -302,6 +356,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d2100.0776999527625!2d1.7371437929129006!3d52.60806141664361!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x0%3A0x20fac8819f2bccc6!2sJoyland!5e1!3m2!1sen!2suk!4v1593791854395!5m2!1sen!2suk</t>
   </si>
   <si>
+    <t>Joyland, Marine Parade, Great Yarmouth NR30 2DL</t>
+  </si>
+  <si>
     <t>Landmark Forest Adventure Park</t>
   </si>
   <si>
@@ -323,6 +380,9 @@
     <t>https://maps.google.co.uk/maps?q=lightwater+valley&amp;oe=utf-8&amp;client=firefox-a&amp;channel=sb&amp;ie=UTF8&amp;hq=&amp;hnear=&amp;ll=54.174546,-1.567484&amp;spn=0.006295,0.006295&amp;t=h&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>Lightwater Valley Family Adventure Park, Water Ln, North Stainley, Ripon HG4 3HT, United Kingdom</t>
+  </si>
+  <si>
     <t>M&amp;D's - Scotland's Theme Park</t>
   </si>
   <si>
@@ -344,6 +404,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d2112.7043485747536!2d-4.802785000000027!3d51.7790460043105!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x48692d0da304ad51%3A0x3b7617f6eb581985!2sOakwood+Theme+Park!5e1!3m2!1sen!2suk!4v1425992256342</t>
   </si>
   <si>
+    <t>Oakwood Theme Park, Canaston Bridge, Narberth SA67 8DE</t>
+  </si>
+  <si>
     <t>Ocean Beach Pleasure Park</t>
   </si>
   <si>
@@ -356,6 +419,9 @@
     <t>https://maps.google.co.uk/maps?f=q&amp;source=s_q&amp;hl=en&amp;geocode=&amp;q=ocean+beach+south+shields&amp;aq=&amp;sll=52.596401,1.735969&amp;sspn=0.014624,0.042272&amp;t=h&amp;ie=UTF8&amp;hq=ocean+beach&amp;hnear=South+Shields,+Tyne+and+Wear,+United+Kingdom&amp;cid=14400602364969143159&amp;ll=55.134145,-1.370544&amp;spn=0.376825,0.878906&amp;z=10&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>Ocean Beach Pleasure Park, Sea Rd, South Shields NE33 2LD, United Kingdom</t>
+  </si>
+  <si>
     <t>Paultons Park - Home of Peppa Pig World</t>
   </si>
   <si>
@@ -368,6 +434,9 @@
     <t>https://googleads.g.doubleclick.net/pagead/ads?gdpr=0&amp;client=ca-pub-1049321617959519&amp;output=html&amp;h=280&amp;adk=2532613036&amp;adf=3527168438&amp;pi=t.aa~a.945740654~i.9~rp.4&amp;w=690&amp;abgtt=3&amp;fwrn=4&amp;fwrnh=100&amp;lmt=1715811730&amp;num_ads=1&amp;rafmt=1&amp;armr=3&amp;sem=mc&amp;pwprc=6765933657&amp;ad_type=text_image&amp;format=690x280&amp;url=https%3A%2F%2Fwww.themeparks-uk.com%2Fuk-theme-parks%2Fengland%2Fpaultons-park-home-of-peppa-pig-world&amp;fwr=0&amp;pra=3&amp;rh=173&amp;rw=690&amp;rpe=1&amp;resp_fmts=3&amp;wgl=1&amp;fa=27&amp;uach=WyJXaW5kb3dzIiwiMTUuMC4wIiwieDg2IiwiIiwiMTI0LjAuNjM2Ny45MSIsbnVsbCwwLG51bGwsIjY0IixbWyJOb3QtQS5CcmFuZCIsIjk5LjAuMC4wIl0sWyJDaHJvbWl1bSIsIjEyNC4wLjYzNjcuOTEiXV0sMF0.&amp;dt=1715811730662&amp;bpp=1&amp;bdt=532&amp;idt=1&amp;shv=r20240513&amp;mjsv=m202405080101&amp;ptt=9&amp;saldr=aa&amp;abxe=1&amp;cookie_enabled=1&amp;eo_id_str=ID%3Db1e8d754f0923851%3AT%3D1715807624%3ART%3D1715808244%3AS%3DAA-AfjZDPJLd_KwhwPZ5sM1wfYvJ&amp;prev_fmts=0x0%2C720x280&amp;nras=3&amp;correlator=4765772976961&amp;frm=20&amp;pv=1&amp;ga_vid=672736908.1715811087&amp;ga_sid=1715811730&amp;ga_hid=178095372&amp;ga_fc=1&amp;u_tz=120&amp;u_his=31&amp;u_h=864&amp;u_w=1536&amp;u_ah=864&amp;u_aw=1536&amp;u_cd=24&amp;u_sd=1&amp;dmc=8&amp;adx=55&amp;ady=912&amp;biw=800&amp;bih=600&amp;scr_x=0&amp;scr_y=0&amp;eid=44759875%2C44759926%2C44759837%2C31083588%2C42531705%2C44795921%2C95331983%2C95332927%2C95331711%2C95332415%2C31078663%2C31078665%2C31078668%2C31078670&amp;oid=2&amp;pvsid=4193121500923960&amp;tmod=1904942740&amp;uas=0&amp;nvt=1&amp;fc=1408&amp;brdim=12%2C12%2C12%2C12%2C1536%2C0%2C1313%2C996%2C800%2C600&amp;vis=1&amp;rsz=%7C%7Cs%7C&amp;abl=NS&amp;fu=128&amp;bc=31&amp;bz=1.64&amp;td=1&amp;psd=W251bGwsbnVsbCxudWxsLDFd&amp;nt=1&amp;ifi=4&amp;uci=a!4&amp;btvi=1&amp;fsb=1&amp;dtd=274</t>
   </si>
   <si>
+    <t>Paultons Park Home of Peppa Pig World, Romsey SO51 6AL, United Kingdom</t>
+  </si>
+  <si>
     <t>Pettitts Animal Adventure Park</t>
   </si>
   <si>
@@ -380,6 +449,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d2359.4707819177393!2d1.5780311696996536!3d52.566929041644485!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x47d758950eb9b8fb%3A0xcf5e446b67a1b1c4!2sPettitts%20Animal%20Adventure%20Park!5e1!3m2!1sen!2suk!4v1594802583215!5m2!1sen!2suk</t>
   </si>
   <si>
+    <t>Pettitts Animal Adventure Park, Church Rd, Reedham, Norwich NR13 3UA</t>
+  </si>
+  <si>
     <t>Pleasurewood Hills</t>
   </si>
   <si>
@@ -392,6 +464,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3064.0320312883173!2d1.7422144159986344!3d52.50703514494215!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x47da1adeac2f3d53%3A0x55699e1db8345f1d!2sPleasurewood%20Hills%20Family%20Theme%20Park!5e1!3m2!1sen!2suk!4v1614628648126!5m2!1sen!2suk</t>
   </si>
   <si>
+    <t>Pleasurewood Hills Family Theme Park, Leisure Way, Lowestoft NR32 5DZ</t>
+  </si>
+  <si>
     <t>ROARR!</t>
   </si>
   <si>
@@ -404,6 +479,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d107054.7806368856!2d1.210883950762591!3d52.662809393329596!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x47d761c14b496045%3A0xf750c4b6fc02f198!2sROARR*21!5e1!3m2!1sen!2suk!4v1708603046713!5m2!1sen!2suk</t>
   </si>
   <si>
+    <t>ROARR!, Lenwade, Norwich NR9 5JE</t>
+  </si>
+  <si>
     <t>Southport Pleasureland</t>
   </si>
   <si>
@@ -416,6 +494,9 @@
     <t>https://maps.google.co.uk/maps?f=q&amp;source=s_q&amp;hl=en&amp;geocode=&amp;q=southport+pleasureland+PR8+1RX&amp;aq=&amp;sll=53.650538,-3.018586&amp;sspn=0.02854,0.084543&amp;t=h&amp;g=Marine+Dr,+Southport+PR8+1RX&amp;ie=UTF8&amp;hq=southport+pleasureland+PR8+1RX&amp;cid=982262478626422838&amp;hnear=&amp;ll=54.297294,-2.828979&amp;spn=1.538778,3.515625&amp;z=8&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>Southport Pleasureland, Marine Dr, Southport PR8 1RX, United Kingdom</t>
+  </si>
+  <si>
     <t>Sundown Adventureland</t>
   </si>
   <si>
@@ -428,6 +509,9 @@
     <t>https://googleads.g.doubleclick.net/pagead/ads?gdpr=0&amp;client=ca-pub-1049321617959519&amp;output=html&amp;h=200&amp;adk=334255576&amp;adf=3527168438&amp;pi=t.aa~a.945740654~i.3~rp.4&amp;w=690&amp;abgtt=3&amp;fwrn=4&amp;fwrnh=100&amp;lmt=1715811815&amp;num_ads=1&amp;rafmt=1&amp;armr=3&amp;sem=mc&amp;pwprc=6765933657&amp;ad_type=text_image&amp;format=690x200&amp;url=https%3A%2F%2Fwww.themeparks-uk.com%2Fuk-theme-parks%2Fengland%2Fsundown-adventureland&amp;fwr=0&amp;pra=3&amp;rh=173&amp;rw=690&amp;rpe=1&amp;resp_fmts=3&amp;wgl=1&amp;fa=27&amp;uach=WyJXaW5kb3dzIiwiMTUuMC4wIiwieDg2IiwiIiwiMTI0LjAuNjM2Ny45MSIsbnVsbCwwLG51bGwsIjY0IixbWyJOb3QtQS5CcmFuZCIsIjk5LjAuMC4wIl0sWyJDaHJvbWl1bSIsIjEyNC4wLjYzNjcuOTEiXV0sMF0.&amp;dt=1715811815769&amp;bpp=1&amp;bdt=422&amp;idt=-M&amp;shv=r20240513&amp;mjsv=m202405080101&amp;ptt=9&amp;saldr=aa&amp;abxe=1&amp;cookie_enabled=1&amp;eo_id_str=ID%3Db1e8d754f0923851%3AT%3D1715807624%3ART%3D1715808244%3AS%3DAA-AfjZDPJLd_KwhwPZ5sM1wfYvJ&amp;prev_fmts=0x0%2C720x280%2C345x280&amp;nras=3&amp;correlator=8517505984543&amp;frm=20&amp;pv=1&amp;ga_vid=672736908.1715811087&amp;ga_sid=1715811815&amp;ga_hid=1533263106&amp;ga_fc=1&amp;u_tz=120&amp;u_his=36&amp;u_h=864&amp;u_w=1536&amp;u_ah=864&amp;u_aw=1536&amp;u_cd=24&amp;u_sd=1&amp;dmc=8&amp;adx=55&amp;ady=743&amp;biw=800&amp;bih=600&amp;scr_x=0&amp;scr_y=0&amp;eid=44759875%2C44759926%2C44759837%2C31083636%2C44795922%2C95331689%2C95331982%2C95331711%2C95332416%2C31078663%2C31078665%2C31078668%2C31078670&amp;oid=2&amp;pvsid=4141813310511342&amp;tmod=697365255&amp;uas=0&amp;nvt=1&amp;fc=1408&amp;brdim=12%2C12%2C12%2C12%2C1536%2C0%2C1313%2C996%2C800%2C600&amp;vis=1&amp;rsz=%7C%7Cs%7C&amp;abl=NS&amp;fu=128&amp;bc=31&amp;bz=1.64&amp;td=1&amp;psd=W251bGwsbnVsbCxudWxsLDFd&amp;nt=1&amp;ifi=4&amp;uci=a!4&amp;btvi=2&amp;fsb=1&amp;dtd=225</t>
   </si>
   <si>
+    <t>Sundown Adventureland, Treswell Rd, Rampton, Retford DN22 0HX</t>
+  </si>
+  <si>
     <t>The Big Sheep</t>
   </si>
   <si>
@@ -440,6 +524,9 @@
     <t>https://www.google.com/maps/embed?pb=!1m17!1m11!1m3!1d1380.2279565984732!2d-4.244093834456374!3d51.015738997331454!2m2!1f0!2f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x486c15fdc9d99b23%3A0x4e58bfa86056d457!2sThe+BIG+Sheep!5e1!3m2!1sen!2suk!4v1476894740356</t>
   </si>
   <si>
+    <t>The BIG Sheep, Abbotsham Rd, Abbotsham, Bideford EX39 5AP</t>
+  </si>
+  <si>
     <t>The Milky Way Adventure Park</t>
   </si>
   <si>
@@ -452,6 +539,9 @@
     <t>https://maps.google.co.uk/maps?q=the+milky+way+adventure+park&amp;oe=utf-8&amp;client=firefox-a&amp;channel=sb&amp;ie=UTF8&amp;hq=&amp;hnear=&amp;ll=50.981776,-4.383716&amp;spn=0.006295,0.006295&amp;t=h&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>The Milky Way Adventure Park, Bideford EX39 5RY, United Kingdom</t>
+  </si>
+  <si>
     <t>Twinlakes</t>
   </si>
   <si>
@@ -482,6 +572,9 @@
     <t>https://maps.google.co.uk/maps?hl=en&amp;client=firefox-a&amp;q=west+midland+safari+park&amp;ie=UTF8&amp;hq=west+midland+safari+park&amp;t=h&amp;cid=11076381864681974024&amp;ll=53.103919,-2.125854&amp;spn=1.583034,3.515625&amp;z=8&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>West Midlands Safari Park, Spring Grove, Bewdley DY12 1LF, United Kingdom</t>
+  </si>
+  <si>
     <t>Wheelgate</t>
   </si>
   <si>
@@ -494,6 +587,9 @@
     <t>https://maps.google.co.uk/maps?q=wheelgate+park&amp;oe=utf-8&amp;client=firefox-a&amp;channel=sb&amp;ie=UTF8&amp;hq=wheelgate+park&amp;t=h&amp;ll=53.109207,-1.065906&amp;spn=0.006295,0.006295&amp;output=embed</t>
   </si>
   <si>
+    <t>Robin Hoods Wheelgate Park, Mansfield Rd, Farnsfield, Newark NG22 8HX, United Kingdom</t>
+  </si>
+  <si>
     <t>Wicksteed Park</t>
   </si>
   <si>
@@ -506,6 +602,9 @@
     <t>https://maps.google.co.uk/maps?q=wicksteed+park&amp;oe=utf-8&amp;client=firefox-a&amp;channel=sb&amp;ie=UTF8&amp;hq=&amp;hnear=&amp;ll=52.385591,-0.710749&amp;spn=0.006295,0.006295&amp;t=h&amp;iwloc=A&amp;output=embed</t>
   </si>
   <si>
+    <t>Wicksteed Park, Barton Rd, Kettering NN15 6NJ, United Kingdom</t>
+  </si>
+  <si>
     <t>Woodlands</t>
   </si>
   <si>
@@ -516,6 +615,9 @@
   </si>
   <si>
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d5378.269271247939!2d-3.674986450954178!3d50.35712075850029!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x486d1ebe4ab8050f%3A0x8fc8b316e73cf54!2sWoodlands+Family+Theme+Park!5e1!3m2!1sen!2suk!4v1553629412224</t>
+  </si>
+  <si>
+    <t>Woodlands Family Theme Park, Woodlands Leisure Park A3122, Blackawton, Totnes TQ9 7DQ</t>
   </si>
 </sst>
 </file>
@@ -979,8 +1081,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ba8bdc96-3af2-4501-89ba-e7fb8e69e3ed}">
-  <dimension ref="A1:D44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{c7beffbe-c5ee-4de3-8fc5-7b167df1b0d8}">
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -989,9 +1091,10 @@
     <col min="1" max="1" width="36.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="84.7142857142857" customWidth="1"/>
     <col min="3" max="4" width="255.714285714286" customWidth="1"/>
+    <col min="5" max="5" width="98.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75">
+    <row r="1" spans="1:5" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1004,581 +1107,713 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="12.75">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="12.75">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="12.75">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="12.75">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="12.75">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="12.75">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="12.75">
+        <v>42</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="12.75">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="12.75">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" ht="12.75">
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="12.75">
+        <v>57</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="12.75">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A15" s="2" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="12.75">
+        <v>67</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="12.75">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>71</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="12.75">
+        <v>75</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="12.75">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A19" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="12.75">
+        <v>85</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="12.75">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A21" s="2" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="12.75">
+        <v>94</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12.75">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>99</v>
+      </c>
+      <c r="E22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A23" s="2" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="12.75">
+        <v>104</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>108</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A25" s="2" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="12.75">
+        <v>112</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12.75">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>116</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A27" s="2" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="12.75">
+        <v>120</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="12.75">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>124</v>
+      </c>
+      <c r="E28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A29" s="2" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="12.75">
+        <v>128</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="12.75">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="D30" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>133</v>
+      </c>
+      <c r="E30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A31" s="2" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="12.75">
+        <v>138</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="12.75">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="D32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>143</v>
+      </c>
+      <c r="E32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A33" s="2" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="12.75">
+        <v>148</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="12.75">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="D34" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>153</v>
+      </c>
+      <c r="E34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A35" s="2" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="12.75">
+        <v>158</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="12.75">
       <c r="A36" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="C36" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>163</v>
+      </c>
+      <c r="E36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A37" s="2" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="12.75">
+        <v>168</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="12.75">
       <c r="A38" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="C38" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>173</v>
+      </c>
+      <c r="E38" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A39" s="2" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:4" ht="12.75">
+      <c r="E39" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="12.75">
       <c r="A40" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="B40" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="C40" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>180</v>
+      </c>
+      <c r="E40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A41" s="2" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="12.75">
+        <v>184</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="12.75">
       <c r="A42" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="B42" t="s">
-        <v>156</v>
+        <v>187</v>
       </c>
       <c r="C42" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="D42" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>189</v>
+      </c>
+      <c r="E42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A43" s="2" t="s">
-        <v>159</v>
+        <v>191</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>160</v>
+        <v>192</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="12.75">
+        <v>194</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="12.75">
       <c r="A44" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="C44" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="D44" t="s">
-        <v>166</v>
+        <v>199</v>
+      </c>
+      <c r="E44" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>